<commit_message>
script update after round 1
</commit_message>
<xml_diff>
--- a/data/ModelParameters.xlsx
+++ b/data/ModelParameters.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\devan.mcgranahan\GithubProjects\Greenstripping\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F730669F-3712-4B61-8DAD-7FC6649B5601}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64CBD8F5-CB3A-4C61-9337-B41CDDFBFD1C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13875" xr2:uid="{B3AEE400-3561-4738-9323-0770B7673F06}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="16">
   <si>
     <t xml:space="preserve">Location </t>
   </si>
@@ -44,9 +44,6 @@
     <t>inches_precip</t>
   </si>
   <si>
-    <t>tons_acre</t>
-  </si>
-  <si>
     <t>ND</t>
   </si>
   <si>
@@ -78,6 +75,12 @@
   </si>
   <si>
     <t>OR</t>
+  </si>
+  <si>
+    <t>lb_acre</t>
+  </si>
+  <si>
+    <t>t/ha</t>
   </si>
 </sst>
 </file>
@@ -429,10 +432,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{38A13DEF-AE4F-4280-8296-0BFF6B19E705}">
-  <dimension ref="A1:C21"/>
+  <dimension ref="A1:D21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -440,7 +443,7 @@
     <col min="2" max="2" width="11.46484375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -448,56 +451,75 @@
         <v>2</v>
       </c>
       <c r="C1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2">
+        <v>12.3</v>
+      </c>
+      <c r="C2">
+        <v>420</v>
+      </c>
+      <c r="D2">
+        <f>C2*0.00112085</f>
+        <v>0.47075700000000004</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>17.600000000000001</v>
-      </c>
-      <c r="C2">
-        <v>1870</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A3" t="s">
-        <v>4</v>
-      </c>
       <c r="B3">
-        <v>15.4</v>
+        <v>16.8</v>
       </c>
       <c r="C3">
-        <v>1680</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.45">
+        <v>470</v>
+      </c>
+      <c r="D3">
+        <f>C3*0.00112085</f>
+        <v>0.52679949999999998</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>12</v>
       </c>
       <c r="B4">
-        <v>16.8</v>
+        <v>12</v>
       </c>
       <c r="C4">
-        <v>1000</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.45">
+        <v>490</v>
+      </c>
+      <c r="D4">
+        <f>C4*0.00112085</f>
+        <v>0.5492165</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>4</v>
       </c>
       <c r="B5">
-        <v>16.8</v>
+        <v>12.5</v>
       </c>
       <c r="C5">
-        <v>470</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.45">
+        <v>500</v>
+      </c>
+      <c r="D5">
+        <f>C5*0.00112085</f>
+        <v>0.56042500000000006</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6">
         <v>16.8</v>
@@ -505,21 +527,29 @@
       <c r="C6">
         <v>530</v>
       </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D6">
+        <f>C6*0.00112085</f>
+        <v>0.59405050000000004</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
+        <v>12</v>
+      </c>
+      <c r="B7">
+        <v>9</v>
+      </c>
+      <c r="C7">
+        <v>620</v>
+      </c>
+      <c r="D7">
+        <f>C7*0.00112085</f>
+        <v>0.69492700000000007</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A8" t="s">
         <v>5</v>
-      </c>
-      <c r="B7">
-        <v>16</v>
-      </c>
-      <c r="C7">
-        <v>1220</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A8" t="s">
-        <v>6</v>
       </c>
       <c r="B8">
         <v>15.7</v>
@@ -527,151 +557,210 @@
       <c r="C8">
         <v>630</v>
       </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.45">
+      <c r="D8">
+        <f>C8*0.00112085</f>
+        <v>0.70613550000000003</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="C9">
+        <v>670</v>
+      </c>
+      <c r="D9">
+        <f>C9*0.00112085</f>
+        <v>0.75096950000000007</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A10" t="s">
+        <v>10</v>
+      </c>
+      <c r="B10">
+        <v>13</v>
+      </c>
+      <c r="C10">
+        <v>680</v>
+      </c>
+      <c r="D10">
+        <f>C10*0.00112085</f>
+        <v>0.76217800000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A11" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11">
+        <v>14</v>
+      </c>
+      <c r="C11">
+        <v>700</v>
+      </c>
+      <c r="D11">
+        <f>C11*0.00112085</f>
+        <v>0.78459500000000004</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A12" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12">
+        <v>13.4</v>
+      </c>
+      <c r="C12">
+        <v>740</v>
+      </c>
+      <c r="D12">
+        <f>C12*0.00112085</f>
+        <v>0.82942900000000008</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13">
+        <v>11.3</v>
+      </c>
+      <c r="C13">
+        <v>810</v>
+      </c>
+      <c r="D13">
+        <f>C13*0.00112085</f>
+        <v>0.9078885000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14">
+        <v>14.9</v>
+      </c>
+      <c r="C14">
+        <v>970</v>
+      </c>
+      <c r="D14">
+        <f>C14*0.00112085</f>
+        <v>1.0872245</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A15" t="s">
+        <v>3</v>
+      </c>
+      <c r="B15">
+        <v>16.8</v>
+      </c>
+      <c r="C15">
+        <v>1000</v>
+      </c>
+      <c r="D15">
+        <f>C15*0.00112085</f>
+        <v>1.1208500000000001</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A16" t="s">
+        <v>4</v>
+      </c>
+      <c r="B16">
+        <v>16</v>
+      </c>
+      <c r="C16">
+        <v>1220</v>
+      </c>
+      <c r="D16">
+        <f>C16*0.00112085</f>
+        <v>1.367437</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A17" t="s">
         <v>7</v>
       </c>
-      <c r="B9">
+      <c r="B17">
+        <v>14.1</v>
+      </c>
+      <c r="C17">
+        <v>1330</v>
+      </c>
+      <c r="D17">
+        <f>C17*0.00112085</f>
+        <v>1.4907305000000002</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18">
         <v>15.5</v>
       </c>
-      <c r="C9">
+      <c r="C18">
         <v>1620</v>
       </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A10" t="s">
-        <v>8</v>
-      </c>
-      <c r="B10">
+      <c r="D18">
+        <f>C18*0.00112085</f>
+        <v>1.8157770000000002</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A19" t="s">
+        <v>3</v>
+      </c>
+      <c r="B19">
+        <v>15.4</v>
+      </c>
+      <c r="C19">
+        <v>1680</v>
+      </c>
+      <c r="D19">
+        <f>C19*0.00112085</f>
+        <v>1.8830280000000001</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A20" t="s">
+        <v>1</v>
+      </c>
+      <c r="B20">
+        <v>17.600000000000001</v>
+      </c>
+      <c r="C20">
+        <v>1870</v>
+      </c>
+      <c r="D20">
+        <f>C20*0.00112085</f>
+        <v>2.0959894999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.45">
+      <c r="A21" t="s">
+        <v>7</v>
+      </c>
+      <c r="B21">
         <v>15.1</v>
       </c>
-      <c r="C10">
+      <c r="C21">
         <v>1870</v>
       </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A11" t="s">
-        <v>7</v>
-      </c>
-      <c r="B11">
-        <v>14.9</v>
-      </c>
-      <c r="C11">
-        <v>970</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A12" t="s">
-        <v>8</v>
-      </c>
-      <c r="B12">
-        <v>14.1</v>
-      </c>
-      <c r="C12">
-        <v>1330</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A13" t="s">
-        <v>9</v>
-      </c>
-      <c r="B13">
-        <v>14</v>
-      </c>
-      <c r="C13">
-        <v>700</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A14" t="s">
-        <v>10</v>
-      </c>
-      <c r="B14">
-        <v>13.4</v>
-      </c>
-      <c r="C14">
-        <v>740</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A15" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15">
-        <v>13</v>
-      </c>
-      <c r="C15">
-        <v>680</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A16" t="s">
-        <v>5</v>
-      </c>
-      <c r="B16">
-        <v>12.5</v>
-      </c>
-      <c r="C16">
-        <v>500</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A17" t="s">
-        <v>12</v>
-      </c>
-      <c r="B17">
-        <v>12.3</v>
-      </c>
-      <c r="C17">
-        <v>420</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A18" t="s">
-        <v>13</v>
-      </c>
-      <c r="B18">
-        <v>12</v>
-      </c>
-      <c r="C18">
-        <v>490</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A19" t="s">
-        <v>14</v>
-      </c>
-      <c r="B19">
-        <v>11.3</v>
-      </c>
-      <c r="C19">
-        <v>810</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A20" t="s">
-        <v>5</v>
-      </c>
-      <c r="B20">
-        <v>9.3000000000000007</v>
-      </c>
-      <c r="C20">
-        <v>670</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.45">
-      <c r="A21" t="s">
-        <v>13</v>
-      </c>
-      <c r="B21">
-        <v>9</v>
-      </c>
-      <c r="C21">
-        <v>620</v>
+      <c r="D21">
+        <f>C21*0.00112085</f>
+        <v>2.0959894999999999</v>
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:D21">
+    <sortCondition ref="D2:D21"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>